<commit_message>
my august final timesheet from the day i started
</commit_message>
<xml_diff>
--- a/neelma_august_timesheet.xlsx
+++ b/neelma_august_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t xml:space="preserve">employee name:</t>
   </si>
@@ -38,6 +38,96 @@
   </si>
   <si>
     <t xml:space="preserve">Hours Worked</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> week</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> week</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> week</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
@@ -140,33 +230,21 @@
     <t xml:space="preserve">20.8.18</t>
   </si>
   <si>
-    <t xml:space="preserve">worked on github started creating repositories learning commands and commiting</t>
+    <t xml:space="preserve">worked on github started creating repositories learning commands and commiting and worked on html created facebook index page.</t>
   </si>
   <si>
     <t xml:space="preserve">21.8.18</t>
   </si>
   <si>
-    <t xml:space="preserve">worked more on html and pushed on github</t>
-  </si>
-  <si>
     <t xml:space="preserve">22.8.18</t>
   </si>
   <si>
-    <t xml:space="preserve">html forms </t>
-  </si>
-  <si>
     <t xml:space="preserve">23.8.18</t>
   </si>
   <si>
-    <t xml:space="preserve">facebook index page</t>
-  </si>
-  <si>
     <t xml:space="preserve">24.8.18</t>
   </si>
   <si>
-    <t xml:space="preserve">started  CSS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total Hours (2nd Week)</t>
   </si>
   <si>
@@ -179,7 +257,7 @@
     <t xml:space="preserve">27.8.18</t>
   </si>
   <si>
-    <t xml:space="preserve">css styling with html</t>
+    <t xml:space="preserve">started CSS </t>
   </si>
   <si>
     <t xml:space="preserve">28.8.18</t>
@@ -228,7 +306,7 @@
     <numFmt numFmtId="169" formatCode="H:MM\ AM/PM"/>
     <numFmt numFmtId="170" formatCode="H:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -266,6 +344,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -480,7 +565,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,7 +657,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,7 +681,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,24 +766,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J50" activeCellId="0" sqref="J50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="44.8163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -811,13 +896,12 @@
     </row>
     <row r="9" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
-      <c r="B9" s="12" t="e">
-        <f aca="false">DATE(YEAR(I4),MONTH(I4),1+0*7)-WEEKDAY(DATE(YEAR(I4),MONTH(I4),8-2))</f>
-        <v>#VALUE!</v>
+      <c r="B9" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="n">
-        <f aca="false">I28</f>
+        <f aca="false">I26</f>
         <v>1.33333333333333</v>
       </c>
       <c r="E9" s="13"/>
@@ -829,14 +913,13 @@
     </row>
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
-      <c r="B10" s="12" t="e">
-        <f aca="false">DATE(YEAR(I4),MONTH(I4),1+1*7)-WEEKDAY(DATE(YEAR(I4),MONTH(I4),8-2))</f>
-        <v>#VALUE!</v>
+      <c r="B10" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="13" t="n">
-        <f aca="false">I38</f>
-        <v>1.66666666666667</v>
+        <f aca="false">I36</f>
+        <v>0.333333333333333</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
@@ -847,13 +930,12 @@
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
-      <c r="B11" s="12" t="e">
-        <f aca="false">DATE(YEAR(I4),MONTH(I4),1+2*7)-WEEKDAY(DATE(YEAR(I4),MONTH(I4),8-2))</f>
-        <v>#VALUE!</v>
+      <c r="B11" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="13" t="n">
-        <f aca="false">I48</f>
+        <f aca="false">I46</f>
         <v>1.66666666666667</v>
       </c>
       <c r="E11" s="13"/>
@@ -863,55 +945,43 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
-      <c r="B12" s="12" t="e">
-        <f aca="false">DATE(YEAR(I4),MONTH(I4),1+3*7)-WEEKDAY(DATE(YEAR(I4),MONTH(I4),8-2))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16" t="n">
+        <f aca="false">SUM(D9:E11)</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
-      <c r="B13" s="12" t="e">
-        <f aca="false">DATE(YEAR(I4),MONTH(I4),1+4*7)-WEEKDAY(DATE(YEAR(I4),MONTH(I4),8-2))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
-      <c r="B14" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16" t="e">
-        <f aca="false">SUM(D9:E13)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -930,7 +1000,9 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -952,88 +1024,108 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="19"/>
+      <c r="B18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="19"/>
+      <c r="B19" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="30" t="n">
+        <f aca="false">(E19-D19)+(H19-G19)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
-      <c r="B20" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="30" t="n">
+        <f aca="false">(E20-D20)+(H20-G20)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="19"/>
       <c r="B21" s="24" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
       <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="26"/>
+      <c r="G21" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H21" s="26" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I21" s="30" t="n">
         <f aca="false">(E21-D21)+(H21-G21)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>16</v>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
       <c r="B22" s="24" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
@@ -1044,17 +1136,17 @@
         <f aca="false">(E22-D22)+(H22-G22)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="31" t="s">
-        <v>16</v>
+      <c r="J22" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="19"/>
       <c r="B23" s="24" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
@@ -1070,41 +1162,45 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
       <c r="B24" s="24" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
       <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="26"/>
+      <c r="G24" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H24" s="26" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I24" s="30" t="n">
         <f aca="false">(E24-D24)+(H24-G24)</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
       <c r="B25" s="24" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="29" t="n">
         <v>0.416666666666667</v>
       </c>
@@ -1116,144 +1212,140 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
-      <c r="B26" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H26" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I26" s="30" t="n">
-        <f aca="false">(E26-D26)+(H26-G26)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="J26" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="36" t="n">
+        <f aca="false">SUM(I19:I25)</f>
+        <v>1.33333333333333</v>
+      </c>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="19"/>
-      <c r="B27" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H27" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I27" s="30" t="n">
-        <f aca="false">(E27-D27)+(H27-G27)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="J27" s="32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="19"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="36" t="n">
-        <f aca="false">SUM(I21:I27)</f>
-        <v>1.33333333333333</v>
-      </c>
-      <c r="J28" s="19"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-    </row>
-    <row r="30" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="30" t="n">
+        <f aca="false">(E29-D29)+(H29-G29)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="19"/>
-      <c r="B30" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="30" t="n">
+        <f aca="false">(E30-D30)+(H30-G30)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="19"/>
       <c r="B31" s="24" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="27"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="26"/>
+      <c r="G31" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H31" s="26" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I31" s="30" t="n">
         <f aca="false">(E31-D31)+(H31-G31)</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J31" s="31" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="19"/>
       <c r="B32" s="24" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
@@ -1264,241 +1356,226 @@
         <f aca="false">(E32-D32)+(H32-G32)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="31" t="s">
-        <v>24</v>
+      <c r="J32" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19"/>
       <c r="B33" s="24" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="27"/>
       <c r="F33" s="28"/>
-      <c r="G33" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H33" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I33" s="30" t="n">
-        <f aca="false">(E33-D33)+(H33-G33)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>39</v>
+      <c r="G33" s="29"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="19"/>
       <c r="B34" s="24" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="27"/>
       <c r="F34" s="28"/>
-      <c r="G34" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H34" s="26" t="n">
-        <v>0.75</v>
-      </c>
+      <c r="G34" s="29"/>
+      <c r="H34" s="26"/>
       <c r="I34" s="30" t="n">
         <f aca="false">(E34-D34)+(H34-G34)</f>
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="19"/>
       <c r="B35" s="24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H35" s="26" t="n">
-        <v>0.75</v>
-      </c>
+      <c r="F35" s="33"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="26"/>
       <c r="I35" s="30" t="n">
         <f aca="false">(E35-D35)+(H35-G35)</f>
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="19"/>
-      <c r="B36" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H36" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I36" s="30" t="n">
-        <f aca="false">(E36-D36)+(H36-G36)</f>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36" s="36" t="n">
+        <f aca="false">SUM(I29:I35)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="J36" s="32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="19"/>
-      <c r="B37" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H37" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I37" s="30" t="n">
-        <f aca="false">(E37-D37)+(H37-G37)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="J37" s="32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="19"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="35" t="s">
+      <c r="B38" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="19"/>
+      <c r="B39" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I38" s="36" t="n">
-        <f aca="false">SUM(I31:I37)</f>
-        <v>1.66666666666667</v>
-      </c>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C39" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="30" t="n">
+        <f aca="false">(E39-D39)+(H39-G39)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="19"/>
-      <c r="B40" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="30" t="n">
+        <f aca="false">(E40-D40)+(H40-G40)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="19"/>
       <c r="B41" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D41" s="26"/>
       <c r="E41" s="27"/>
       <c r="F41" s="28"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="26"/>
+      <c r="G41" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H41" s="26" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I41" s="30" t="n">
         <f aca="false">(E41-D41)+(H41-G41)</f>
-        <v>0</v>
-      </c>
-      <c r="J41" s="31" t="s">
-        <v>24</v>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="19"/>
       <c r="B42" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="27"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="26"/>
+      <c r="G42" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H42" s="26" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I42" s="30" t="n">
         <f aca="false">(E42-D42)+(H42-G42)</f>
-        <v>0</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>24</v>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="19"/>
       <c r="B43" s="24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="27"/>
@@ -1514,16 +1591,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="19"/>
       <c r="B44" s="24" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D44" s="26"/>
       <c r="E44" s="27"/>
@@ -1539,20 +1616,20 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J44" s="32" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="19"/>
       <c r="B45" s="24" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D45" s="26"/>
       <c r="E45" s="27"/>
-      <c r="F45" s="28"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="29" t="n">
         <v>0.416666666666667</v>
       </c>
@@ -1564,77 +1641,51 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J45" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="19"/>
-      <c r="B46" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H46" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I46" s="30" t="n">
-        <f aca="false">(E46-D46)+(H46-G46)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="J46" s="32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="I46" s="36" t="n">
+        <f aca="false">SUM(I39:I45)</f>
+        <v>1.66666666666667</v>
+      </c>
+      <c r="J46" s="19"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="19"/>
-      <c r="B47" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="29" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="H47" s="26" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I47" s="30" t="n">
-        <f aca="false">(E47-D47)+(H47-G47)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="J47" s="32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="19"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="I48" s="36" t="n">
-        <f aca="false">SUM(I41:I47)</f>
-        <v>1.66666666666667</v>
-      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
       <c r="J48" s="19"/>
     </row>
-    <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
@@ -1646,69 +1697,69 @@
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
     </row>
-    <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-    </row>
-    <row r="51" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="40"/>
+    </row>
+    <row r="51" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
+      <c r="B51" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-    </row>
-    <row r="52" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H51" s="43"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="40"/>
+    </row>
+    <row r="52" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="37"/>
+      <c r="B52" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
       <c r="F52" s="37"/>
       <c r="G52" s="37"/>
       <c r="H52" s="38"/>
-      <c r="I52" s="39"/>
+      <c r="I52" s="45"/>
       <c r="J52" s="40"/>
     </row>
-    <row r="53" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="19"/>
-      <c r="B53" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="44"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="40"/>
       <c r="J53" s="40"/>
     </row>
-    <row r="54" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="19"/>
-      <c r="B54" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="45"/>
-      <c r="J54" s="40"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="19"/>
@@ -1718,59 +1769,59 @@
       <c r="E55" s="19"/>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-    </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-    </row>
-    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+    </row>
+    <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="46"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="48"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1779,34 +1830,10 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="J62" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="21">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:F4"/>
@@ -1827,13 +1854,7 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D51:E51"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>